<commit_message>
update template and data_to_excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rew\PycharmProjects\CCI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C6A6EA-D2C0-4565-8AD3-E707B50046E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4747A17A-43FD-4326-9BC9-7F27F80277F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-24" windowWidth="23256" windowHeight="12456" xr2:uid="{9771F661-60CA-46B0-9189-DCE67C33EAEF}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27030" windowHeight="14130" xr2:uid="{9771F661-60CA-46B0-9189-DCE67C33EAEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Zone</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -96,6 +96,26 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>KR-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RYU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RUNNING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>STOP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>HDD(GB)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -108,10 +128,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>/dev/mapper/VG01-app : /app 100G</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>SWAP(GB)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>External</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>API</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -120,13 +148,25 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>192.
-192.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/data
-/data2</t>
+    <t>CentOS 7.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>111.111.111.111</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.25.1.20
+172.25.2.30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>111.111.111.113</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.25.1.21
+172.25.2.31</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -134,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,16 +224,8 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,14 +274,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -258,10 +284,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -274,12 +311,62 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -291,51 +378,63 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,173 +750,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF3F7C4-2CEB-4626-AE15-B65C84588A9C}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.75" style="3"/>
-    <col min="8" max="8" width="8.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="34.25" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.5" style="3" customWidth="1"/>
-    <col min="13" max="13" width="15" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="8.75" style="3"/>
+    <col min="1" max="1" width="5.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.75" style="1"/>
+    <col min="10" max="10" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="13" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="14"/>
+      <c r="O1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="10"/>
+      <c r="P1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>100</v>
+      </c>
+      <c r="J4" s="2">
+        <v>200</v>
+      </c>
+      <c r="K4" s="2">
+        <v>500</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3">
+        <v>45492</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:16" ht="33" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>200</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="3">
+        <v>45492</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:15" ht="33" x14ac:dyDescent="0.3">
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>19</v>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="F1:K1"/>
+  <mergeCells count="17">
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="F1:L1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add customer variable template.xlsx, data_to_excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rew\PycharmProjects\CCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4315A1ED-61DC-4627-8D1E-0114EAA8FE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA410047-F5FE-420C-AAE5-9F7141DAC129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-24" windowWidth="23256" windowHeight="12456" xr2:uid="{9771F661-60CA-46B0-9189-DCE67C33EAEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9771F661-60CA-46B0-9189-DCE67C33EAEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Zone</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>External</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서생성날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객명</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -215,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -312,13 +324,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -339,6 +360,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -687,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF3F7C4-2CEB-4626-AE15-B65C84588A9C}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -715,120 +739,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="10"/>
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="O2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="11"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="2"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="18"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -848,25 +868,45 @@
       <c r="O5" s="3"/>
       <c r="P5" s="2"/>
     </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
+  <mergeCells count="19">
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="O1:P1"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:K3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>